<commit_message>
components page has been added
</commit_message>
<xml_diff>
--- a/target/test-classes/com/opencart/TestData/TestDataOpenCart.xlsx
+++ b/target/test-classes/com/opencart/TestData/TestDataOpenCart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piyush ramteke\eclipse-workspace\opencart\src\test\java\com\opencart\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196D2F6E-BCA4-46FC-80B3-78BD6F260855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB08654-6AE2-4CB1-BE7A-DD42F1C0251D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F8F0743C-B4FD-4D2B-A602-E069D8ECEEF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>rteg45&amp;</t>
+  </si>
+  <si>
+    <t>mno@gmail.com</t>
+  </si>
+  <si>
+    <t>tervvv&amp;</t>
+  </si>
+  <si>
+    <t>bpu@yahoo.in</t>
+  </si>
+  <si>
+    <t>ygegge7</t>
   </si>
 </sst>
 </file>
@@ -131,12 +143,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -452,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F478B6E4-3B9E-4035-A0B6-80387F65DDB7}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,10 +492,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -494,6 +505,22 @@
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -502,8 +529,10 @@
     <hyperlink ref="A4" r:id="rId2" xr:uid="{26756D1C-F6B1-4ECF-A84E-34BF05CC67B3}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{8A9BA661-E1C6-4980-8E7F-0953A1E3822A}"/>
     <hyperlink ref="A3" r:id="rId4" xr:uid="{B8F0C9A4-8447-4D95-881B-E222CA7FA334}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{E8AABCCE-6E62-4B93-A0E9-6AA06DC86F34}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{770B48FF-382A-4D60-BED1-213D60C88776}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>